<commit_message>
execel files to check
</commit_message>
<xml_diff>
--- a/mainproduct.xlsx
+++ b/mainproduct.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="146">
   <si>
     <t xml:space="preserve">Product Name</t>
   </si>
@@ -43,10 +43,28 @@
     <t xml:space="preserve">image_url</t>
   </si>
   <si>
-    <t xml:space="preserve">Custom Field Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Custom Field Value</t>
+    <t xml:space="preserve">Custom Field Name1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Field Name2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Field Name3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Field Name4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Field Value1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Field Value2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Field Value3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Field Value4</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -232,7 +250,25 @@
     <t xml:space="preserve">color</t>
   </si>
   <si>
+    <t xml:space="preserve">custcolor2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">custcolor3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">custcolor4</t>
+  </si>
+  <si>
     <t xml:space="preserve">red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cred3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cred4</t>
   </si>
   <si>
     <t xml:space="preserve">string</t>
@@ -296,9 +332,27 @@
     <t xml:space="preserve">weight</t>
   </si>
   <si>
+    <t xml:space="preserve">custweight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">custweight3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">custweight4</t>
+  </si>
+  <si>
     <t xml:space="preserve">10kg</t>
   </si>
   <si>
+    <t xml:space="preserve">c10kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c10kg3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c10kg4</t>
+  </si>
+  <si>
     <t xml:space="preserve">warranty2</t>
   </si>
   <si>
@@ -329,9 +383,27 @@
     <t xml:space="preserve">height</t>
   </si>
   <si>
+    <t xml:space="preserve">custheight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">custheight3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">custheight4</t>
+  </si>
+  <si>
     <t xml:space="preserve">100cm</t>
   </si>
   <si>
+    <t xml:space="preserve">c100cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c100cm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c100cm4</t>
+  </si>
+  <si>
     <t xml:space="preserve">warranty3</t>
   </si>
   <si>
@@ -351,6 +423,42 @@
   </si>
   <si>
     <t xml:space="preserve">videodescription3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECTROLITE 3.0 TRAVEL SPINNER 55CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sk111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;&lt;span&gt;Meet Spectrolite 3.0 Trvl Spinner 55cm by Samsonite. Offering the highest level of organisation and security, Spectrolite 3.0 TRVL is the perfect choice for business travellers. This collection brings you smart features, durability and thoughtfully designed interiors to ensure optimal packing comfort. Its tech-inspired design is in perfect match with our Spectrolite 3.0 business bag&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn11.bigcommerce.com/s-b5ajmj9rbq/product_images/uploaded_images/product1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATERIAL INFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZIPPERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HANDLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHEEL HANDLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Softside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Top &amp; side handles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double tube</t>
   </si>
 </sst>
 </file>
@@ -359,14 +467,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -382,18 +489,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -444,7 +539,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -465,14 +560,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,47 +577,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BM5"/>
+  <dimension ref="A1:BS5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AS1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AY8" activeCellId="0" sqref="AY8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="23.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="19.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="0" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="29.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="54" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="57" style="0" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="29.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="60" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="15.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -558,25 +648,25 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="0" t="s">
@@ -729,16 +819,34 @@
       <c r="BM1" s="0" t="s">
         <v>64</v>
       </c>
+      <c r="BN1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="0" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>137260</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>175</v>
@@ -747,192 +855,219 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="0" t="n">
+      <c r="R2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="T2" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="U2" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="V2" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="W2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="X2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="S2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="T2" s="0" t="n">
+      <c r="Y2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="AA2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="V2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="W2" s="0" t="n">
+      <c r="AB2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="X2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>71</v>
+      <c r="AD2" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AE2" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AF2" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI2" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO2" s="0" t="n">
         <v>-2147483648</v>
       </c>
-      <c r="AJ2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="0" t="n">
+      <c r="AP2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ2" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AR2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AM2" s="0" t="n">
+      <c r="AS2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AN2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ2" s="0" t="n">
+      <c r="AT2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV2" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AW2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AR2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="AS2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AU2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AW2" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="AX2" s="0" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="AY2" s="0" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="AZ2" s="3" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="BA2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="BD2" s="3" t="s">
-        <v>71</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BB2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD2" s="0" t="s">
+        <v>83</v>
       </c>
       <c r="BE2" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="BF2" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="BF2" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BG2" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BH2" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BI2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BJ2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BK2" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="BL2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="BG2" s="0" t="n">
+      <c r="BM2" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="BH2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="BI2" s="0" t="n">
+      <c r="BN2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="BO2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="BJ2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="BK2" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="BL2" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="BM2" s="0" t="s">
-        <v>85</v>
+      <c r="BP2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="BQ2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="BR2" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="BS2" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>200</v>
@@ -941,192 +1076,219 @@
         <v>24</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>68</v>
+        <v>101</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K3" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="R3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="S3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="T3" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="U3" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="V3" s="0" t="n">
         <v>101</v>
       </c>
-      <c r="Q3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U3" s="0" t="n">
+      <c r="W3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="V3" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="W3" s="0" t="n">
+      <c r="AB3" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC3" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="X3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AD3" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AE3" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AF3" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AG3" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK3" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL3" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <v>-2147483647</v>
+      </c>
+      <c r="AP3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ3" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AR3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV3" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AW3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AY3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AZ3" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BA3" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BB3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC3" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="BD3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="BE3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="BF3" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BG3" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BH3" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BI3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BJ3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BK3" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="AB3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE3" s="0" t="s">
+      <c r="BL3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="BM3" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="BN3" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="AF3" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH3" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI3" s="0" t="n">
-        <v>-2147483647</v>
-      </c>
-      <c r="AJ3" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN3" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP3" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="AQ3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR3" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AU3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AV3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AW3" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AY3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AZ3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="BA3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="BD3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="BE3" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="BF3" s="0" t="n">
+      <c r="BO3" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="BG3" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="BH3" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="BI3" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="BJ3" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="BK3" s="0" t="s">
+      <c r="BP3" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="BQ3" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="BR3" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="BS3" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="BL3" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="BM3" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2323</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>300</v>
@@ -1135,191 +1297,315 @@
         <v>20</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="I4" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="V4" s="0" t="n">
         <v>102</v>
       </c>
-      <c r="K4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>202</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <v>102</v>
-      </c>
-      <c r="Q4" s="0" t="n">
+      <c r="W4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="X4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="S4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="T4" s="0" t="n">
+      <c r="Y4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="AA4" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="V4" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="W4" s="0" t="n">
+      <c r="AB4" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC4" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="X4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE4" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="AF4" s="0" t="s">
-        <v>74</v>
+      <c r="AD4" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AE4" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AF4" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="AG4" s="0" t="s">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="AH4" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI4" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="AI4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK4" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO4" s="0" t="n">
         <v>-2147483646</v>
       </c>
-      <c r="AJ4" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="0" t="n">
+      <c r="AP4" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ4" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AR4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AM4" s="0" t="n">
+      <c r="AS4" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="AN4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP4" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="AQ4" s="0" t="n">
+      <c r="AT4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV4" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AW4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AR4" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="AS4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AU4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AV4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AW4" s="0" t="s">
-        <v>106</v>
-      </c>
       <c r="AX4" s="0" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="AY4" s="0" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="AZ4" s="3" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="BA4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="BD4" s="3" t="s">
-        <v>71</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BB4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC4" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD4" s="0" t="s">
+        <v>83</v>
       </c>
       <c r="BE4" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="BF4" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="BF4" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BG4" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BH4" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BI4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BJ4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BK4" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="BL4" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="BG4" s="0" t="n">
+      <c r="BM4" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="BH4" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="BI4" s="0" t="n">
+      <c r="BN4" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="BO4" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="BJ4" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="BK4" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="BL4" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="BM4" s="0" t="s">
-        <v>85</v>
+      <c r="BP4" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="BQ4" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="BR4" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="BS4" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AU5" s="3"/>
+      <c r="A5" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>799</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB5" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AD5" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AE5" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AF5" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="BA5" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="https://cdn11.bigcommerce.com/s-b5ajmj9rbq/product_images/uploaded_images/graybag.jpeg"/>
     <hyperlink ref="G3" r:id="rId2" display="https://cdn11.bigcommerce.com/s-b5ajmj9rbq/product_images/uploaded_images/graybag.jpeg"/>
     <hyperlink ref="G4" r:id="rId3" display="https://cdn11.bigcommerce.com/s-b5ajmj9rbq/product_images/uploaded_images/graybag.jpeg"/>
+    <hyperlink ref="G5" r:id="rId4" display="https://cdn11.bigcommerce.com/s-b5ajmj9rbq/product_images/uploaded_images/product1.jpg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>